<commit_message>
created a sample cpp file for all files.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1672,7 +1672,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1791,7 +1791,7 @@
         <v>14</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
common elements in 3 sorted arrays
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1687,7 +1687,7 @@
       <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.34"/>
@@ -1985,7 +1985,7 @@
         <v>31</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
find subarray with sum 0
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1684,7 +1684,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B8" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.0859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2013,7 +2013,7 @@
         <v>33</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Find factorial of large numbers
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1684,7 +1684,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B8" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.0859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2027,7 +2027,7 @@
         <v>34</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
find triplet that sums to a particular number.
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="472">
   <si>
     <t xml:space="preserve">Questions by Love Babbar:</t>
   </si>
@@ -1683,8 +1683,8 @@
   </sheetPr>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B8" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B20" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2111,7 +2111,7 @@
         <v>40</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2138,9 +2138,7 @@
       <c r="C35" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">

</xml_diff>

<commit_message>
minimum length subarray with sum greater than x
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1681,7 +1681,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B23" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2150,7 +2150,7 @@
         <v>42</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
median in row-wise sorted matrix
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\vineet\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812A1FA5-788D-4BBF-AF87-579D0EBEC875}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABD0994-0C83-4A76-A04A-CF528305353B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1927,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
@@ -2517,7 +2517,7 @@
         <v>51</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="21">

</xml_diff>

<commit_message>
find row with max 1s
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\vineet\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABD0994-0C83-4A76-A04A-CF528305353B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DB8E27-E07C-4482-A57C-B87B11E2C9D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1928,7 +1928,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
@@ -2529,7 +2529,7 @@
         <v>52</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="21">

</xml_diff>

<commit_message>
sort elements in matrix
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\vineet\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DB8E27-E07C-4482-A57C-B87B11E2C9D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CFCBD6-0980-4C0D-B520-CFE2AFD35858}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1928,7 +1928,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
@@ -2541,7 +2541,7 @@
         <v>53</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Added numbering in the list topic wise
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\vineet\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CFCBD6-0980-4C0D-B520-CFE2AFD35858}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B8210E-E961-4279-90F9-A8F83298B217}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1927,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A271" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B472" sqref="B472:B481"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
@@ -2488,7 +2488,9 @@
       <c r="A44" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="6"/>
+      <c r="B44" s="6">
+        <v>1</v>
+      </c>
       <c r="C44" s="7" t="s">
         <v>49</v>
       </c>
@@ -2500,7 +2502,9 @@
       <c r="A45" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="6"/>
+      <c r="B45" s="6">
+        <v>2</v>
+      </c>
       <c r="C45" s="7" t="s">
         <v>50</v>
       </c>
@@ -2512,7 +2516,9 @@
       <c r="A46" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="6"/>
+      <c r="B46" s="6">
+        <v>3</v>
+      </c>
       <c r="C46" s="7" t="s">
         <v>51</v>
       </c>
@@ -2524,7 +2530,9 @@
       <c r="A47" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="6"/>
+      <c r="B47" s="6">
+        <v>4</v>
+      </c>
       <c r="C47" s="7" t="s">
         <v>52</v>
       </c>
@@ -2536,7 +2544,9 @@
       <c r="A48" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="6"/>
+      <c r="B48" s="6">
+        <v>5</v>
+      </c>
       <c r="C48" s="7" t="s">
         <v>53</v>
       </c>
@@ -2548,7 +2558,9 @@
       <c r="A49" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="6"/>
+      <c r="B49" s="6">
+        <v>6</v>
+      </c>
       <c r="C49" s="7" t="s">
         <v>54</v>
       </c>
@@ -2560,7 +2572,9 @@
       <c r="A50" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="6"/>
+      <c r="B50" s="6">
+        <v>7</v>
+      </c>
       <c r="C50" s="7" t="s">
         <v>55</v>
       </c>
@@ -2572,7 +2586,9 @@
       <c r="A51" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="6"/>
+      <c r="B51" s="6">
+        <v>8</v>
+      </c>
       <c r="C51" s="7" t="s">
         <v>56</v>
       </c>
@@ -2584,7 +2600,9 @@
       <c r="A52" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B52" s="6"/>
+      <c r="B52" s="6">
+        <v>9</v>
+      </c>
       <c r="C52" s="7" t="s">
         <v>57</v>
       </c>
@@ -2592,11 +2610,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="21">
+    <row r="53" spans="1:4" ht="17.25" customHeight="1">
       <c r="A53" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="6"/>
+      <c r="B53" s="6">
+        <v>10</v>
+      </c>
       <c r="C53" s="7" t="s">
         <v>58</v>
       </c>
@@ -2614,7 +2634,9 @@
       <c r="A56" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B56" s="6"/>
+      <c r="B56" s="6">
+        <v>1</v>
+      </c>
       <c r="C56" s="7" t="s">
         <v>60</v>
       </c>
@@ -2626,7 +2648,9 @@
       <c r="A57" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="6"/>
+      <c r="B57" s="6">
+        <v>2</v>
+      </c>
       <c r="C57" s="7" t="s">
         <v>61</v>
       </c>
@@ -2638,7 +2662,9 @@
       <c r="A58" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B58" s="6"/>
+      <c r="B58" s="6">
+        <v>3</v>
+      </c>
       <c r="C58" s="7" t="s">
         <v>62</v>
       </c>
@@ -2650,7 +2676,9 @@
       <c r="A59" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="6"/>
+      <c r="B59" s="6">
+        <v>4</v>
+      </c>
       <c r="C59" s="8" t="s">
         <v>63</v>
       </c>
@@ -2662,7 +2690,9 @@
       <c r="A60" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B60" s="6"/>
+      <c r="B60" s="6">
+        <v>5</v>
+      </c>
       <c r="C60" s="7" t="s">
         <v>64</v>
       </c>
@@ -2674,7 +2704,9 @@
       <c r="A61" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B61" s="6"/>
+      <c r="B61" s="6">
+        <v>6</v>
+      </c>
       <c r="C61" s="7" t="s">
         <v>65</v>
       </c>
@@ -2686,7 +2718,9 @@
       <c r="A62" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B62" s="6"/>
+      <c r="B62" s="6">
+        <v>7</v>
+      </c>
       <c r="C62" s="7" t="s">
         <v>66</v>
       </c>
@@ -2698,7 +2732,9 @@
       <c r="A63" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B63" s="6"/>
+      <c r="B63" s="6">
+        <v>8</v>
+      </c>
       <c r="C63" s="7" t="s">
         <v>67</v>
       </c>
@@ -2710,7 +2746,9 @@
       <c r="A64" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B64" s="6"/>
+      <c r="B64" s="6">
+        <v>9</v>
+      </c>
       <c r="C64" s="7" t="s">
         <v>68</v>
       </c>
@@ -2722,7 +2760,9 @@
       <c r="A65" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B65" s="6"/>
+      <c r="B65" s="6">
+        <v>10</v>
+      </c>
       <c r="C65" s="7" t="s">
         <v>69</v>
       </c>
@@ -2734,7 +2774,9 @@
       <c r="A66" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B66" s="6"/>
+      <c r="B66" s="6">
+        <v>11</v>
+      </c>
       <c r="C66" s="7" t="s">
         <v>70</v>
       </c>
@@ -2746,7 +2788,9 @@
       <c r="A67" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B67" s="6"/>
+      <c r="B67" s="6">
+        <v>12</v>
+      </c>
       <c r="C67" s="7" t="s">
         <v>71</v>
       </c>
@@ -2758,7 +2802,9 @@
       <c r="A68" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B68" s="6"/>
+      <c r="B68" s="6">
+        <v>13</v>
+      </c>
       <c r="C68" s="7" t="s">
         <v>72</v>
       </c>
@@ -2770,7 +2816,9 @@
       <c r="A69" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B69" s="6"/>
+      <c r="B69" s="6">
+        <v>14</v>
+      </c>
       <c r="C69" s="7" t="s">
         <v>73</v>
       </c>
@@ -2782,7 +2830,9 @@
       <c r="A70" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B70" s="6"/>
+      <c r="B70" s="6">
+        <v>15</v>
+      </c>
       <c r="C70" s="7" t="s">
         <v>74</v>
       </c>
@@ -2794,7 +2844,9 @@
       <c r="A71" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B71" s="6"/>
+      <c r="B71" s="6">
+        <v>16</v>
+      </c>
       <c r="C71" s="7" t="s">
         <v>75</v>
       </c>
@@ -2806,7 +2858,9 @@
       <c r="A72" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B72" s="6"/>
+      <c r="B72" s="6">
+        <v>17</v>
+      </c>
       <c r="C72" s="7" t="s">
         <v>76</v>
       </c>
@@ -2818,7 +2872,9 @@
       <c r="A73" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B73" s="6"/>
+      <c r="B73" s="6">
+        <v>18</v>
+      </c>
       <c r="C73" s="7" t="s">
         <v>77</v>
       </c>
@@ -2830,7 +2886,9 @@
       <c r="A74" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B74" s="6"/>
+      <c r="B74" s="6">
+        <v>19</v>
+      </c>
       <c r="C74" s="7" t="s">
         <v>78</v>
       </c>
@@ -2842,7 +2900,9 @@
       <c r="A75" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B75" s="6"/>
+      <c r="B75" s="6">
+        <v>20</v>
+      </c>
       <c r="C75" s="7" t="s">
         <v>79</v>
       </c>
@@ -2854,7 +2914,9 @@
       <c r="A76" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B76" s="6"/>
+      <c r="B76" s="6">
+        <v>21</v>
+      </c>
       <c r="C76" s="7" t="s">
         <v>80</v>
       </c>
@@ -2866,7 +2928,9 @@
       <c r="A77" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B77" s="6"/>
+      <c r="B77" s="6">
+        <v>22</v>
+      </c>
       <c r="C77" s="7" t="s">
         <v>81</v>
       </c>
@@ -2878,7 +2942,9 @@
       <c r="A78" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B78" s="6"/>
+      <c r="B78" s="6">
+        <v>23</v>
+      </c>
       <c r="C78" s="7" t="s">
         <v>82</v>
       </c>
@@ -2890,7 +2956,9 @@
       <c r="A79" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B79" s="6"/>
+      <c r="B79" s="6">
+        <v>24</v>
+      </c>
       <c r="C79" s="7" t="s">
         <v>83</v>
       </c>
@@ -2902,7 +2970,9 @@
       <c r="A80" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B80" s="6"/>
+      <c r="B80" s="6">
+        <v>25</v>
+      </c>
       <c r="C80" s="7" t="s">
         <v>84</v>
       </c>
@@ -2914,7 +2984,9 @@
       <c r="A81" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B81" s="6"/>
+      <c r="B81" s="6">
+        <v>26</v>
+      </c>
       <c r="C81" s="7" t="s">
         <v>85</v>
       </c>
@@ -2926,7 +2998,9 @@
       <c r="A82" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B82" s="6"/>
+      <c r="B82" s="6">
+        <v>27</v>
+      </c>
       <c r="C82" s="7" t="s">
         <v>86</v>
       </c>
@@ -2938,7 +3012,9 @@
       <c r="A83" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B83" s="6"/>
+      <c r="B83" s="6">
+        <v>28</v>
+      </c>
       <c r="C83" s="7" t="s">
         <v>87</v>
       </c>
@@ -2950,7 +3026,9 @@
       <c r="A84" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B84" s="6"/>
+      <c r="B84" s="6">
+        <v>29</v>
+      </c>
       <c r="C84" s="7" t="s">
         <v>88</v>
       </c>
@@ -2962,7 +3040,9 @@
       <c r="A85" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B85" s="6"/>
+      <c r="B85" s="6">
+        <v>30</v>
+      </c>
       <c r="C85" s="7" t="s">
         <v>89</v>
       </c>
@@ -2974,7 +3054,9 @@
       <c r="A86" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B86" s="6"/>
+      <c r="B86" s="6">
+        <v>31</v>
+      </c>
       <c r="C86" s="7" t="s">
         <v>90</v>
       </c>
@@ -2986,7 +3068,9 @@
       <c r="A87" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B87" s="6"/>
+      <c r="B87" s="6">
+        <v>32</v>
+      </c>
       <c r="C87" s="7" t="s">
         <v>91</v>
       </c>
@@ -2998,7 +3082,9 @@
       <c r="A88" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B88" s="6"/>
+      <c r="B88" s="6">
+        <v>33</v>
+      </c>
       <c r="C88" s="7" t="s">
         <v>92</v>
       </c>
@@ -3010,7 +3096,9 @@
       <c r="A89" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B89" s="6"/>
+      <c r="B89" s="6">
+        <v>34</v>
+      </c>
       <c r="C89" s="7" t="s">
         <v>93</v>
       </c>
@@ -3022,7 +3110,9 @@
       <c r="A90" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B90" s="6"/>
+      <c r="B90" s="6">
+        <v>35</v>
+      </c>
       <c r="C90" s="7" t="s">
         <v>94</v>
       </c>
@@ -3034,7 +3124,9 @@
       <c r="A91" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B91" s="6"/>
+      <c r="B91" s="6">
+        <v>36</v>
+      </c>
       <c r="C91" s="7" t="s">
         <v>95</v>
       </c>
@@ -3046,7 +3138,9 @@
       <c r="A92" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B92" s="6"/>
+      <c r="B92" s="6">
+        <v>37</v>
+      </c>
       <c r="C92" s="7" t="s">
         <v>96</v>
       </c>
@@ -3058,7 +3152,9 @@
       <c r="A93" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B93" s="6"/>
+      <c r="B93" s="6">
+        <v>38</v>
+      </c>
       <c r="C93" s="7" t="s">
         <v>97</v>
       </c>
@@ -3070,7 +3166,9 @@
       <c r="A94" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B94" s="6"/>
+      <c r="B94" s="6">
+        <v>39</v>
+      </c>
       <c r="C94" s="7" t="s">
         <v>98</v>
       </c>
@@ -3082,7 +3180,9 @@
       <c r="A95" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B95" s="6"/>
+      <c r="B95" s="6">
+        <v>40</v>
+      </c>
       <c r="C95" s="7" t="s">
         <v>99</v>
       </c>
@@ -3094,7 +3194,9 @@
       <c r="A96" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B96" s="6"/>
+      <c r="B96" s="6">
+        <v>41</v>
+      </c>
       <c r="C96" s="7" t="s">
         <v>100</v>
       </c>
@@ -3106,7 +3208,9 @@
       <c r="A97" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B97" s="6"/>
+      <c r="B97" s="6">
+        <v>42</v>
+      </c>
       <c r="C97" s="7" t="s">
         <v>101</v>
       </c>
@@ -3118,7 +3222,9 @@
       <c r="A98" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B98" s="6"/>
+      <c r="B98" s="6">
+        <v>43</v>
+      </c>
       <c r="C98" s="7" t="s">
         <v>102</v>
       </c>
@@ -3136,7 +3242,9 @@
       <c r="A101" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B101" s="6"/>
+      <c r="B101" s="6">
+        <v>1</v>
+      </c>
       <c r="C101" s="7" t="s">
         <v>104</v>
       </c>
@@ -3148,7 +3256,9 @@
       <c r="A102" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B102" s="6"/>
+      <c r="B102" s="6">
+        <v>2</v>
+      </c>
       <c r="C102" s="7" t="s">
         <v>105</v>
       </c>
@@ -3160,7 +3270,9 @@
       <c r="A103" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B103" s="6"/>
+      <c r="B103" s="6">
+        <v>3</v>
+      </c>
       <c r="C103" s="7" t="s">
         <v>106</v>
       </c>
@@ -3172,7 +3284,9 @@
       <c r="A104" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B104" s="6"/>
+      <c r="B104" s="6">
+        <v>4</v>
+      </c>
       <c r="C104" s="7" t="s">
         <v>107</v>
       </c>
@@ -3184,7 +3298,9 @@
       <c r="A105" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B105" s="6"/>
+      <c r="B105" s="6">
+        <v>5</v>
+      </c>
       <c r="C105" s="7" t="s">
         <v>108</v>
       </c>
@@ -3196,7 +3312,9 @@
       <c r="A106" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B106" s="6"/>
+      <c r="B106" s="6">
+        <v>6</v>
+      </c>
       <c r="C106" s="7" t="s">
         <v>109</v>
       </c>
@@ -3208,7 +3326,9 @@
       <c r="A107" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B107" s="6"/>
+      <c r="B107" s="6">
+        <v>7</v>
+      </c>
       <c r="C107" s="7" t="s">
         <v>110</v>
       </c>
@@ -3220,7 +3340,9 @@
       <c r="A108" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B108" s="6"/>
+      <c r="B108" s="6">
+        <v>8</v>
+      </c>
       <c r="C108" s="7" t="s">
         <v>111</v>
       </c>
@@ -3232,7 +3354,9 @@
       <c r="A109" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B109" s="6"/>
+      <c r="B109" s="6">
+        <v>9</v>
+      </c>
       <c r="C109" s="7" t="s">
         <v>112</v>
       </c>
@@ -3244,7 +3368,9 @@
       <c r="A110" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B110" s="6"/>
+      <c r="B110" s="6">
+        <v>10</v>
+      </c>
       <c r="C110" s="7" t="s">
         <v>113</v>
       </c>
@@ -3256,7 +3382,9 @@
       <c r="A111" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B111" s="6"/>
+      <c r="B111" s="6">
+        <v>11</v>
+      </c>
       <c r="C111" s="7" t="s">
         <v>114</v>
       </c>
@@ -3268,7 +3396,9 @@
       <c r="A112" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B112" s="6"/>
+      <c r="B112" s="6">
+        <v>12</v>
+      </c>
       <c r="C112" s="7" t="s">
         <v>115</v>
       </c>
@@ -3280,7 +3410,9 @@
       <c r="A113" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B113" s="6"/>
+      <c r="B113" s="6">
+        <v>13</v>
+      </c>
       <c r="C113" s="7" t="s">
         <v>116</v>
       </c>
@@ -3292,7 +3424,9 @@
       <c r="A114" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B114" s="6"/>
+      <c r="B114" s="6">
+        <v>14</v>
+      </c>
       <c r="C114" s="7" t="s">
         <v>117</v>
       </c>
@@ -3304,7 +3438,9 @@
       <c r="A115" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B115" s="6"/>
+      <c r="B115" s="6">
+        <v>15</v>
+      </c>
       <c r="C115" s="7" t="s">
         <v>118</v>
       </c>
@@ -3316,7 +3452,9 @@
       <c r="A116" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B116" s="6"/>
+      <c r="B116" s="6">
+        <v>16</v>
+      </c>
       <c r="C116" s="7" t="s">
         <v>119</v>
       </c>
@@ -3328,7 +3466,9 @@
       <c r="A117" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B117" s="6"/>
+      <c r="B117" s="6">
+        <v>17</v>
+      </c>
       <c r="C117" s="7" t="s">
         <v>120</v>
       </c>
@@ -3340,7 +3480,9 @@
       <c r="A118" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B118" s="6"/>
+      <c r="B118" s="6">
+        <v>18</v>
+      </c>
       <c r="C118" s="7" t="s">
         <v>121</v>
       </c>
@@ -3352,7 +3494,9 @@
       <c r="A119" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B119" s="6"/>
+      <c r="B119" s="6">
+        <v>19</v>
+      </c>
       <c r="C119" s="7" t="s">
         <v>122</v>
       </c>
@@ -3364,7 +3508,9 @@
       <c r="A120" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B120" s="6"/>
+      <c r="B120" s="6">
+        <v>20</v>
+      </c>
       <c r="C120" s="7" t="s">
         <v>123</v>
       </c>
@@ -3376,7 +3522,9 @@
       <c r="A121" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B121" s="6"/>
+      <c r="B121" s="6">
+        <v>21</v>
+      </c>
       <c r="C121" s="7" t="s">
         <v>124</v>
       </c>
@@ -3388,7 +3536,9 @@
       <c r="A122" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B122" s="6"/>
+      <c r="B122" s="6">
+        <v>22</v>
+      </c>
       <c r="C122" s="7" t="s">
         <v>125</v>
       </c>
@@ -3400,7 +3550,9 @@
       <c r="A123" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B123" s="6"/>
+      <c r="B123" s="6">
+        <v>23</v>
+      </c>
       <c r="C123" s="7" t="s">
         <v>126</v>
       </c>
@@ -3412,7 +3564,9 @@
       <c r="A124" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B124" s="6"/>
+      <c r="B124" s="6">
+        <v>24</v>
+      </c>
       <c r="C124" s="7" t="s">
         <v>127</v>
       </c>
@@ -3424,7 +3578,9 @@
       <c r="A125" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B125" s="6"/>
+      <c r="B125" s="6">
+        <v>25</v>
+      </c>
       <c r="C125" s="7" t="s">
         <v>128</v>
       </c>
@@ -3436,7 +3592,9 @@
       <c r="A126" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B126" s="6"/>
+      <c r="B126" s="6">
+        <v>26</v>
+      </c>
       <c r="C126" s="7" t="s">
         <v>129</v>
       </c>
@@ -3448,7 +3606,9 @@
       <c r="A127" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B127" s="6"/>
+      <c r="B127" s="6">
+        <v>27</v>
+      </c>
       <c r="C127" s="7" t="s">
         <v>130</v>
       </c>
@@ -3460,7 +3620,9 @@
       <c r="A128" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B128" s="6"/>
+      <c r="B128" s="6">
+        <v>28</v>
+      </c>
       <c r="C128" s="7" t="s">
         <v>131</v>
       </c>
@@ -3472,7 +3634,9 @@
       <c r="A129" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B129" s="6"/>
+      <c r="B129" s="6">
+        <v>29</v>
+      </c>
       <c r="C129" s="7" t="s">
         <v>132</v>
       </c>
@@ -3484,7 +3648,9 @@
       <c r="A130" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B130" s="6"/>
+      <c r="B130" s="6">
+        <v>30</v>
+      </c>
       <c r="C130" s="7" t="s">
         <v>133</v>
       </c>
@@ -3496,7 +3662,9 @@
       <c r="A131" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B131" s="6"/>
+      <c r="B131" s="6">
+        <v>31</v>
+      </c>
       <c r="C131" s="7" t="s">
         <v>134</v>
       </c>
@@ -3508,7 +3676,9 @@
       <c r="A132" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B132" s="6"/>
+      <c r="B132" s="6">
+        <v>32</v>
+      </c>
       <c r="C132" s="7" t="s">
         <v>135</v>
       </c>
@@ -3520,7 +3690,9 @@
       <c r="A133" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B133" s="6"/>
+      <c r="B133" s="6">
+        <v>33</v>
+      </c>
       <c r="C133" s="7" t="s">
         <v>136</v>
       </c>
@@ -3532,7 +3704,9 @@
       <c r="A134" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B134" s="6"/>
+      <c r="B134" s="6">
+        <v>34</v>
+      </c>
       <c r="C134" s="7" t="s">
         <v>137</v>
       </c>
@@ -3544,7 +3718,9 @@
       <c r="A135" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B135" s="6"/>
+      <c r="B135" s="6">
+        <v>35</v>
+      </c>
       <c r="C135" s="7" t="s">
         <v>138</v>
       </c>
@@ -3556,7 +3732,9 @@
       <c r="A136" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B136" s="6"/>
+      <c r="B136" s="6">
+        <v>36</v>
+      </c>
       <c r="C136" s="7" t="s">
         <v>139</v>
       </c>
@@ -3572,7 +3750,9 @@
       <c r="A139" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B139" s="6"/>
+      <c r="B139" s="6">
+        <v>1</v>
+      </c>
       <c r="C139" s="7" t="s">
         <v>141</v>
       </c>
@@ -3584,7 +3764,9 @@
       <c r="A140" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B140" s="6"/>
+      <c r="B140" s="6">
+        <v>2</v>
+      </c>
       <c r="C140" s="7" t="s">
         <v>142</v>
       </c>
@@ -3596,7 +3778,9 @@
       <c r="A141" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B141" s="6"/>
+      <c r="B141" s="6">
+        <v>3</v>
+      </c>
       <c r="C141" s="7" t="s">
         <v>143</v>
       </c>
@@ -3608,7 +3792,9 @@
       <c r="A142" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B142" s="6"/>
+      <c r="B142" s="6">
+        <v>4</v>
+      </c>
       <c r="C142" s="7" t="s">
         <v>144</v>
       </c>
@@ -3620,7 +3806,9 @@
       <c r="A143" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B143" s="6"/>
+      <c r="B143" s="6">
+        <v>5</v>
+      </c>
       <c r="C143" s="7" t="s">
         <v>145</v>
       </c>
@@ -3632,7 +3820,9 @@
       <c r="A144" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B144" s="6"/>
+      <c r="B144" s="6">
+        <v>6</v>
+      </c>
       <c r="C144" s="7" t="s">
         <v>146</v>
       </c>
@@ -3644,7 +3834,9 @@
       <c r="A145" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B145" s="6"/>
+      <c r="B145" s="6">
+        <v>7</v>
+      </c>
       <c r="C145" s="7" t="s">
         <v>147</v>
       </c>
@@ -3656,7 +3848,9 @@
       <c r="A146" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B146" s="6"/>
+      <c r="B146" s="6">
+        <v>8</v>
+      </c>
       <c r="C146" s="7" t="s">
         <v>148</v>
       </c>
@@ -3668,7 +3862,9 @@
       <c r="A147" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B147" s="6"/>
+      <c r="B147" s="6">
+        <v>9</v>
+      </c>
       <c r="C147" s="7" t="s">
         <v>149</v>
       </c>
@@ -3680,7 +3876,9 @@
       <c r="A148" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B148" s="6"/>
+      <c r="B148" s="6">
+        <v>10</v>
+      </c>
       <c r="C148" s="7" t="s">
         <v>150</v>
       </c>
@@ -3692,7 +3890,9 @@
       <c r="A149" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B149" s="6"/>
+      <c r="B149" s="6">
+        <v>11</v>
+      </c>
       <c r="C149" s="7" t="s">
         <v>151</v>
       </c>
@@ -3704,7 +3904,9 @@
       <c r="A150" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B150" s="6"/>
+      <c r="B150" s="6">
+        <v>12</v>
+      </c>
       <c r="C150" s="7" t="s">
         <v>152</v>
       </c>
@@ -3716,7 +3918,9 @@
       <c r="A151" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B151" s="6"/>
+      <c r="B151" s="6">
+        <v>13</v>
+      </c>
       <c r="C151" s="7" t="s">
         <v>153</v>
       </c>
@@ -3728,7 +3932,9 @@
       <c r="A152" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B152" s="6"/>
+      <c r="B152" s="6">
+        <v>14</v>
+      </c>
       <c r="C152" s="7" t="s">
         <v>154</v>
       </c>
@@ -3740,7 +3946,9 @@
       <c r="A153" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B153" s="6"/>
+      <c r="B153" s="6">
+        <v>15</v>
+      </c>
       <c r="C153" s="7" t="s">
         <v>155</v>
       </c>
@@ -3752,7 +3960,9 @@
       <c r="A154" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B154" s="6"/>
+      <c r="B154" s="6">
+        <v>16</v>
+      </c>
       <c r="C154" s="7" t="s">
         <v>156</v>
       </c>
@@ -3764,7 +3974,9 @@
       <c r="A155" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B155" s="6"/>
+      <c r="B155" s="6">
+        <v>17</v>
+      </c>
       <c r="C155" s="7" t="s">
         <v>157</v>
       </c>
@@ -3776,7 +3988,9 @@
       <c r="A156" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B156" s="6"/>
+      <c r="B156" s="6">
+        <v>18</v>
+      </c>
       <c r="C156" s="7" t="s">
         <v>158</v>
       </c>
@@ -3788,7 +4002,9 @@
       <c r="A157" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B157" s="6"/>
+      <c r="B157" s="6">
+        <v>19</v>
+      </c>
       <c r="C157" s="7" t="s">
         <v>159</v>
       </c>
@@ -3800,7 +4016,9 @@
       <c r="A158" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B158" s="6"/>
+      <c r="B158" s="6">
+        <v>20</v>
+      </c>
       <c r="C158" s="7" t="s">
         <v>160</v>
       </c>
@@ -3812,7 +4030,9 @@
       <c r="A159" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B159" s="6"/>
+      <c r="B159" s="6">
+        <v>21</v>
+      </c>
       <c r="C159" s="7" t="s">
         <v>161</v>
       </c>
@@ -3824,7 +4044,9 @@
       <c r="A160" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B160" s="6"/>
+      <c r="B160" s="6">
+        <v>22</v>
+      </c>
       <c r="C160" s="7" t="s">
         <v>162</v>
       </c>
@@ -3836,7 +4058,9 @@
       <c r="A161" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B161" s="6"/>
+      <c r="B161" s="6">
+        <v>23</v>
+      </c>
       <c r="C161" s="7" t="s">
         <v>163</v>
       </c>
@@ -3848,7 +4072,9 @@
       <c r="A162" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B162" s="6"/>
+      <c r="B162" s="6">
+        <v>24</v>
+      </c>
       <c r="C162" s="7" t="s">
         <v>164</v>
       </c>
@@ -3860,7 +4086,9 @@
       <c r="A163" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B163" s="6"/>
+      <c r="B163" s="6">
+        <v>25</v>
+      </c>
       <c r="C163" s="7" t="s">
         <v>165</v>
       </c>
@@ -3872,7 +4100,9 @@
       <c r="A164" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B164" s="6"/>
+      <c r="B164" s="6">
+        <v>26</v>
+      </c>
       <c r="C164" s="8" t="s">
         <v>166</v>
       </c>
@@ -3884,7 +4114,9 @@
       <c r="A165" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B165" s="6"/>
+      <c r="B165" s="6">
+        <v>27</v>
+      </c>
       <c r="C165" s="8" t="s">
         <v>167</v>
       </c>
@@ -3896,7 +4128,9 @@
       <c r="A166" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B166" s="6"/>
+      <c r="B166" s="6">
+        <v>28</v>
+      </c>
       <c r="C166" s="7" t="s">
         <v>168</v>
       </c>
@@ -3908,7 +4142,9 @@
       <c r="A167" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B167" s="6"/>
+      <c r="B167" s="6">
+        <v>29</v>
+      </c>
       <c r="C167" s="7" t="s">
         <v>169</v>
       </c>
@@ -3920,7 +4156,9 @@
       <c r="A168" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B168" s="6"/>
+      <c r="B168" s="6">
+        <v>30</v>
+      </c>
       <c r="C168" s="7" t="s">
         <v>170</v>
       </c>
@@ -3932,7 +4170,9 @@
       <c r="A169" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B169" s="6"/>
+      <c r="B169" s="6">
+        <v>31</v>
+      </c>
       <c r="C169" s="7" t="s">
         <v>171</v>
       </c>
@@ -3944,7 +4184,9 @@
       <c r="A170" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B170" s="6"/>
+      <c r="B170" s="6">
+        <v>32</v>
+      </c>
       <c r="C170" s="7" t="s">
         <v>172</v>
       </c>
@@ -3956,7 +4198,9 @@
       <c r="A171" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B171" s="6"/>
+      <c r="B171" s="6">
+        <v>33</v>
+      </c>
       <c r="C171" s="7" t="s">
         <v>173</v>
       </c>
@@ -3968,7 +4212,9 @@
       <c r="A172" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B172" s="6"/>
+      <c r="B172" s="6">
+        <v>34</v>
+      </c>
       <c r="C172" s="7" t="s">
         <v>174</v>
       </c>
@@ -3980,7 +4226,9 @@
       <c r="A173" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B173" s="6"/>
+      <c r="B173" s="6">
+        <v>35</v>
+      </c>
       <c r="C173" s="7" t="s">
         <v>175</v>
       </c>
@@ -3992,7 +4240,9 @@
       <c r="A174" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B174" s="6"/>
+      <c r="B174" s="6">
+        <v>36</v>
+      </c>
       <c r="C174" s="7" t="s">
         <v>176</v>
       </c>
@@ -4008,7 +4258,9 @@
       <c r="A177" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B177" s="6"/>
+      <c r="B177" s="6">
+        <v>1</v>
+      </c>
       <c r="C177" s="7" t="s">
         <v>178</v>
       </c>
@@ -4020,7 +4272,9 @@
       <c r="A178" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B178" s="6"/>
+      <c r="B178" s="6">
+        <v>2</v>
+      </c>
       <c r="C178" s="7" t="s">
         <v>179</v>
       </c>
@@ -4032,7 +4286,9 @@
       <c r="A179" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B179" s="6"/>
+      <c r="B179" s="6">
+        <v>3</v>
+      </c>
       <c r="C179" s="7" t="s">
         <v>180</v>
       </c>
@@ -4044,7 +4300,9 @@
       <c r="A180" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B180" s="6"/>
+      <c r="B180" s="6">
+        <v>4</v>
+      </c>
       <c r="C180" s="7" t="s">
         <v>181</v>
       </c>
@@ -4056,7 +4314,9 @@
       <c r="A181" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B181" s="6"/>
+      <c r="B181" s="6">
+        <v>5</v>
+      </c>
       <c r="C181" s="7" t="s">
         <v>183</v>
       </c>
@@ -4068,7 +4328,9 @@
       <c r="A182" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B182" s="6"/>
+      <c r="B182" s="6">
+        <v>6</v>
+      </c>
       <c r="C182" s="7" t="s">
         <v>184</v>
       </c>
@@ -4080,7 +4342,9 @@
       <c r="A183" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B183" s="6"/>
+      <c r="B183" s="6">
+        <v>7</v>
+      </c>
       <c r="C183" s="7" t="s">
         <v>185</v>
       </c>
@@ -4092,7 +4356,9 @@
       <c r="A184" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B184" s="6"/>
+      <c r="B184" s="6">
+        <v>8</v>
+      </c>
       <c r="C184" s="7" t="s">
         <v>186</v>
       </c>
@@ -4104,7 +4370,9 @@
       <c r="A185" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B185" s="6"/>
+      <c r="B185" s="6">
+        <v>9</v>
+      </c>
       <c r="C185" s="7" t="s">
         <v>187</v>
       </c>
@@ -4116,7 +4384,9 @@
       <c r="A186" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B186" s="6"/>
+      <c r="B186" s="6">
+        <v>10</v>
+      </c>
       <c r="C186" s="7" t="s">
         <v>188</v>
       </c>
@@ -4128,7 +4398,9 @@
       <c r="A187" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B187" s="6"/>
+      <c r="B187" s="6">
+        <v>11</v>
+      </c>
       <c r="C187" s="7" t="s">
         <v>189</v>
       </c>
@@ -4140,7 +4412,9 @@
       <c r="A188" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B188" s="6"/>
+      <c r="B188" s="6">
+        <v>12</v>
+      </c>
       <c r="C188" s="7" t="s">
         <v>190</v>
       </c>
@@ -4152,7 +4426,9 @@
       <c r="A189" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B189" s="6"/>
+      <c r="B189" s="6">
+        <v>13</v>
+      </c>
       <c r="C189" s="7" t="s">
         <v>191</v>
       </c>
@@ -4164,7 +4440,9 @@
       <c r="A190" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B190" s="6"/>
+      <c r="B190" s="6">
+        <v>14</v>
+      </c>
       <c r="C190" s="7" t="s">
         <v>192</v>
       </c>
@@ -4176,7 +4454,9 @@
       <c r="A191" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B191" s="6"/>
+      <c r="B191" s="6">
+        <v>15</v>
+      </c>
       <c r="C191" s="7" t="s">
         <v>193</v>
       </c>
@@ -4188,7 +4468,9 @@
       <c r="A192" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B192" s="6"/>
+      <c r="B192" s="6">
+        <v>16</v>
+      </c>
       <c r="C192" s="7" t="s">
         <v>194</v>
       </c>
@@ -4200,7 +4482,9 @@
       <c r="A193" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B193" s="6"/>
+      <c r="B193" s="6">
+        <v>17</v>
+      </c>
       <c r="C193" s="7" t="s">
         <v>195</v>
       </c>
@@ -4212,7 +4496,9 @@
       <c r="A194" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B194" s="6"/>
+      <c r="B194" s="6">
+        <v>18</v>
+      </c>
       <c r="C194" s="7" t="s">
         <v>196</v>
       </c>
@@ -4224,7 +4510,9 @@
       <c r="A195" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B195" s="6"/>
+      <c r="B195" s="6">
+        <v>19</v>
+      </c>
       <c r="C195" s="7" t="s">
         <v>197</v>
       </c>
@@ -4236,7 +4524,9 @@
       <c r="A196" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B196" s="6"/>
+      <c r="B196" s="6">
+        <v>20</v>
+      </c>
       <c r="C196" s="7" t="s">
         <v>198</v>
       </c>
@@ -4248,7 +4538,9 @@
       <c r="A197" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B197" s="6"/>
+      <c r="B197" s="6">
+        <v>21</v>
+      </c>
       <c r="C197" s="7" t="s">
         <v>199</v>
       </c>
@@ -4260,7 +4552,9 @@
       <c r="A198" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B198" s="6"/>
+      <c r="B198" s="6">
+        <v>22</v>
+      </c>
       <c r="C198" s="7" t="s">
         <v>200</v>
       </c>
@@ -4272,7 +4566,9 @@
       <c r="A199" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B199" s="6"/>
+      <c r="B199" s="6">
+        <v>23</v>
+      </c>
       <c r="C199" s="7" t="s">
         <v>201</v>
       </c>
@@ -4284,7 +4580,9 @@
       <c r="A200" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B200" s="6"/>
+      <c r="B200" s="6">
+        <v>24</v>
+      </c>
       <c r="C200" s="7" t="s">
         <v>202</v>
       </c>
@@ -4296,7 +4594,9 @@
       <c r="A201" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B201" s="6"/>
+      <c r="B201" s="6">
+        <v>25</v>
+      </c>
       <c r="C201" s="7" t="s">
         <v>203</v>
       </c>
@@ -4308,7 +4608,9 @@
       <c r="A202" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B202" s="6"/>
+      <c r="B202" s="6">
+        <v>26</v>
+      </c>
       <c r="C202" s="7" t="s">
         <v>204</v>
       </c>
@@ -4320,7 +4622,9 @@
       <c r="A203" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B203" s="6"/>
+      <c r="B203" s="6">
+        <v>27</v>
+      </c>
       <c r="C203" s="7" t="s">
         <v>205</v>
       </c>
@@ -4332,7 +4636,9 @@
       <c r="A204" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B204" s="6"/>
+      <c r="B204" s="6">
+        <v>28</v>
+      </c>
       <c r="C204" s="7" t="s">
         <v>206</v>
       </c>
@@ -4344,7 +4650,9 @@
       <c r="A205" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B205" s="6"/>
+      <c r="B205" s="6">
+        <v>29</v>
+      </c>
       <c r="C205" s="7" t="s">
         <v>207</v>
       </c>
@@ -4356,7 +4664,9 @@
       <c r="A206" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B206" s="6"/>
+      <c r="B206" s="6">
+        <v>30</v>
+      </c>
       <c r="C206" s="7" t="s">
         <v>208</v>
       </c>
@@ -4368,7 +4678,9 @@
       <c r="A207" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B207" s="6"/>
+      <c r="B207" s="6">
+        <v>31</v>
+      </c>
       <c r="C207" s="7" t="s">
         <v>209</v>
       </c>
@@ -4380,7 +4692,9 @@
       <c r="A208" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B208" s="6"/>
+      <c r="B208" s="6">
+        <v>32</v>
+      </c>
       <c r="C208" s="7" t="s">
         <v>210</v>
       </c>
@@ -4392,7 +4706,9 @@
       <c r="A209" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B209" s="6"/>
+      <c r="B209" s="6">
+        <v>33</v>
+      </c>
       <c r="C209" s="7" t="s">
         <v>211</v>
       </c>
@@ -4404,7 +4720,9 @@
       <c r="A210" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B210" s="6"/>
+      <c r="B210" s="6">
+        <v>34</v>
+      </c>
       <c r="C210" s="7" t="s">
         <v>212</v>
       </c>
@@ -4416,7 +4734,9 @@
       <c r="A211" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B211" s="6"/>
+      <c r="B211" s="6">
+        <v>35</v>
+      </c>
       <c r="C211" s="7" t="s">
         <v>213</v>
       </c>
@@ -4440,7 +4760,9 @@
       <c r="A214" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B214" s="6"/>
+      <c r="B214" s="6">
+        <v>1</v>
+      </c>
       <c r="C214" s="7" t="s">
         <v>215</v>
       </c>
@@ -4452,7 +4774,9 @@
       <c r="A215" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B215" s="6"/>
+      <c r="B215" s="6">
+        <v>2</v>
+      </c>
       <c r="C215" s="7" t="s">
         <v>216</v>
       </c>
@@ -4464,7 +4788,9 @@
       <c r="A216" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B216" s="6"/>
+      <c r="B216" s="6">
+        <v>3</v>
+      </c>
       <c r="C216" s="7" t="s">
         <v>217</v>
       </c>
@@ -4476,7 +4802,9 @@
       <c r="A217" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B217" s="6"/>
+      <c r="B217" s="6">
+        <v>4</v>
+      </c>
       <c r="C217" s="7" t="s">
         <v>218</v>
       </c>
@@ -4488,7 +4816,9 @@
       <c r="A218" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B218" s="6"/>
+      <c r="B218" s="6">
+        <v>5</v>
+      </c>
       <c r="C218" s="7" t="s">
         <v>219</v>
       </c>
@@ -4500,7 +4830,9 @@
       <c r="A219" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B219" s="6"/>
+      <c r="B219" s="6">
+        <v>6</v>
+      </c>
       <c r="C219" s="7" t="s">
         <v>220</v>
       </c>
@@ -4512,7 +4844,9 @@
       <c r="A220" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B220" s="6"/>
+      <c r="B220" s="6">
+        <v>7</v>
+      </c>
       <c r="C220" s="9" t="s">
         <v>221</v>
       </c>
@@ -4524,7 +4858,9 @@
       <c r="A221" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B221" s="6"/>
+      <c r="B221" s="6">
+        <v>8</v>
+      </c>
       <c r="C221" s="7" t="s">
         <v>222</v>
       </c>
@@ -4536,7 +4872,9 @@
       <c r="A222" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B222" s="6"/>
+      <c r="B222" s="6">
+        <v>9</v>
+      </c>
       <c r="C222" s="7" t="s">
         <v>223</v>
       </c>
@@ -4548,7 +4886,9 @@
       <c r="A223" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B223" s="6"/>
+      <c r="B223" s="6">
+        <v>10</v>
+      </c>
       <c r="C223" s="7" t="s">
         <v>224</v>
       </c>
@@ -4560,7 +4900,9 @@
       <c r="A224" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B224" s="6"/>
+      <c r="B224" s="6">
+        <v>11</v>
+      </c>
       <c r="C224" s="7" t="s">
         <v>225</v>
       </c>
@@ -4572,7 +4914,9 @@
       <c r="A225" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B225" s="6"/>
+      <c r="B225" s="6">
+        <v>12</v>
+      </c>
       <c r="C225" s="7" t="s">
         <v>226</v>
       </c>
@@ -4584,7 +4928,9 @@
       <c r="A226" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B226" s="6"/>
+      <c r="B226" s="6">
+        <v>13</v>
+      </c>
       <c r="C226" s="7" t="s">
         <v>227</v>
       </c>
@@ -4596,7 +4942,9 @@
       <c r="A227" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B227" s="6"/>
+      <c r="B227" s="6">
+        <v>14</v>
+      </c>
       <c r="C227" s="7" t="s">
         <v>228</v>
       </c>
@@ -4608,7 +4956,9 @@
       <c r="A228" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B228" s="6"/>
+      <c r="B228" s="6">
+        <v>15</v>
+      </c>
       <c r="C228" s="7" t="s">
         <v>229</v>
       </c>
@@ -4620,7 +4970,9 @@
       <c r="A229" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B229" s="6"/>
+      <c r="B229" s="6">
+        <v>16</v>
+      </c>
       <c r="C229" s="7" t="s">
         <v>230</v>
       </c>
@@ -4632,7 +4984,9 @@
       <c r="A230" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B230" s="6"/>
+      <c r="B230" s="6">
+        <v>17</v>
+      </c>
       <c r="C230" s="7" t="s">
         <v>231</v>
       </c>
@@ -4644,7 +4998,9 @@
       <c r="A231" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B231" s="6"/>
+      <c r="B231" s="6">
+        <v>18</v>
+      </c>
       <c r="C231" s="7" t="s">
         <v>232</v>
       </c>
@@ -4656,7 +5012,9 @@
       <c r="A232" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B232" s="6"/>
+      <c r="B232" s="6">
+        <v>19</v>
+      </c>
       <c r="C232" s="7" t="s">
         <v>233</v>
       </c>
@@ -4668,7 +5026,9 @@
       <c r="A233" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B233" s="6"/>
+      <c r="B233" s="6">
+        <v>20</v>
+      </c>
       <c r="C233" s="7" t="s">
         <v>234</v>
       </c>
@@ -4680,7 +5040,9 @@
       <c r="A234" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B234" s="6"/>
+      <c r="B234" s="6">
+        <v>21</v>
+      </c>
       <c r="C234" s="7" t="s">
         <v>235</v>
       </c>
@@ -4692,7 +5054,9 @@
       <c r="A235" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B235" s="6"/>
+      <c r="B235" s="6">
+        <v>22</v>
+      </c>
       <c r="C235" s="7" t="s">
         <v>236</v>
       </c>
@@ -4712,7 +5076,9 @@
       <c r="A238" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B238" s="6"/>
+      <c r="B238" s="6">
+        <v>1</v>
+      </c>
       <c r="C238" s="7" t="s">
         <v>238</v>
       </c>
@@ -4724,7 +5090,9 @@
       <c r="A239" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B239" s="6"/>
+      <c r="B239" s="6">
+        <v>2</v>
+      </c>
       <c r="C239" s="7" t="s">
         <v>239</v>
       </c>
@@ -4736,7 +5104,9 @@
       <c r="A240" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B240" s="6"/>
+      <c r="B240" s="6">
+        <v>3</v>
+      </c>
       <c r="C240" s="7" t="s">
         <v>240</v>
       </c>
@@ -4748,7 +5118,9 @@
       <c r="A241" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B241" s="6"/>
+      <c r="B241" s="6">
+        <v>4</v>
+      </c>
       <c r="C241" s="7" t="s">
         <v>241</v>
       </c>
@@ -4760,7 +5132,9 @@
       <c r="A242" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B242" s="6"/>
+      <c r="B242" s="6">
+        <v>5</v>
+      </c>
       <c r="C242" s="7" t="s">
         <v>242</v>
       </c>
@@ -4772,7 +5146,9 @@
       <c r="A243" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B243" s="6"/>
+      <c r="B243" s="6">
+        <v>6</v>
+      </c>
       <c r="C243" s="7" t="s">
         <v>243</v>
       </c>
@@ -4784,7 +5160,9 @@
       <c r="A244" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B244" s="6"/>
+      <c r="B244" s="6">
+        <v>7</v>
+      </c>
       <c r="C244" s="7" t="s">
         <v>244</v>
       </c>
@@ -4796,7 +5174,9 @@
       <c r="A245" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B245" s="6"/>
+      <c r="B245" s="6">
+        <v>8</v>
+      </c>
       <c r="C245" s="7" t="s">
         <v>245</v>
       </c>
@@ -4808,7 +5188,9 @@
       <c r="A246" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B246" s="6"/>
+      <c r="B246" s="6">
+        <v>9</v>
+      </c>
       <c r="C246" s="7" t="s">
         <v>246</v>
       </c>
@@ -4820,7 +5202,9 @@
       <c r="A247" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B247" s="6"/>
+      <c r="B247" s="6">
+        <v>10</v>
+      </c>
       <c r="C247" s="7" t="s">
         <v>247</v>
       </c>
@@ -4832,7 +5216,9 @@
       <c r="A248" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B248" s="6"/>
+      <c r="B248" s="6">
+        <v>11</v>
+      </c>
       <c r="C248" s="7" t="s">
         <v>248</v>
       </c>
@@ -4844,7 +5230,9 @@
       <c r="A249" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B249" s="6"/>
+      <c r="B249" s="6">
+        <v>12</v>
+      </c>
       <c r="C249" s="7" t="s">
         <v>249</v>
       </c>
@@ -4856,7 +5244,9 @@
       <c r="A250" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B250" s="6"/>
+      <c r="B250" s="6">
+        <v>13</v>
+      </c>
       <c r="C250" s="7" t="s">
         <v>250</v>
       </c>
@@ -4868,7 +5258,9 @@
       <c r="A251" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B251" s="6"/>
+      <c r="B251" s="6">
+        <v>14</v>
+      </c>
       <c r="C251" s="7" t="s">
         <v>251</v>
       </c>
@@ -4880,7 +5272,9 @@
       <c r="A252" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B252" s="6"/>
+      <c r="B252" s="6">
+        <v>15</v>
+      </c>
       <c r="C252" s="7" t="s">
         <v>252</v>
       </c>
@@ -4892,7 +5286,9 @@
       <c r="A253" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B253" s="6"/>
+      <c r="B253" s="6">
+        <v>16</v>
+      </c>
       <c r="C253" s="7" t="s">
         <v>253</v>
       </c>
@@ -4904,7 +5300,9 @@
       <c r="A254" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B254" s="6"/>
+      <c r="B254" s="6">
+        <v>17</v>
+      </c>
       <c r="C254" s="7" t="s">
         <v>254</v>
       </c>
@@ -4916,7 +5314,9 @@
       <c r="A255" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B255" s="6"/>
+      <c r="B255" s="6">
+        <v>18</v>
+      </c>
       <c r="C255" s="7" t="s">
         <v>255</v>
       </c>
@@ -4928,7 +5328,9 @@
       <c r="A256" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B256" s="6"/>
+      <c r="B256" s="6">
+        <v>19</v>
+      </c>
       <c r="C256" s="7" t="s">
         <v>256</v>
       </c>
@@ -4940,7 +5342,9 @@
       <c r="A257" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B257" s="6"/>
+      <c r="B257" s="6">
+        <v>20</v>
+      </c>
       <c r="C257" s="7" t="s">
         <v>257</v>
       </c>
@@ -4952,7 +5356,9 @@
       <c r="A258" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B258" s="6"/>
+      <c r="B258" s="6">
+        <v>21</v>
+      </c>
       <c r="C258" s="7" t="s">
         <v>258</v>
       </c>
@@ -4964,7 +5370,9 @@
       <c r="A259" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B259" s="6"/>
+      <c r="B259" s="6">
+        <v>22</v>
+      </c>
       <c r="C259" s="7" t="s">
         <v>259</v>
       </c>
@@ -4976,7 +5384,9 @@
       <c r="A260" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B260" s="6"/>
+      <c r="B260" s="6">
+        <v>23</v>
+      </c>
       <c r="C260" s="7" t="s">
         <v>260</v>
       </c>
@@ -4988,7 +5398,9 @@
       <c r="A261" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B261" s="6"/>
+      <c r="B261" s="6">
+        <v>24</v>
+      </c>
       <c r="C261" s="7" t="s">
         <v>261</v>
       </c>
@@ -5000,7 +5412,9 @@
       <c r="A262" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B262" s="6"/>
+      <c r="B262" s="6">
+        <v>25</v>
+      </c>
       <c r="C262" s="7" t="s">
         <v>262</v>
       </c>
@@ -5012,7 +5426,9 @@
       <c r="A263" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B263" s="6"/>
+      <c r="B263" s="6">
+        <v>26</v>
+      </c>
       <c r="C263" s="7" t="s">
         <v>263</v>
       </c>
@@ -5024,7 +5440,9 @@
       <c r="A264" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B264" s="6"/>
+      <c r="B264" s="6">
+        <v>27</v>
+      </c>
       <c r="C264" s="7" t="s">
         <v>264</v>
       </c>
@@ -5036,7 +5454,9 @@
       <c r="A265" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B265" s="6"/>
+      <c r="B265" s="6">
+        <v>28</v>
+      </c>
       <c r="C265" s="7" t="s">
         <v>265</v>
       </c>
@@ -5048,7 +5468,9 @@
       <c r="A266" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B266" s="6"/>
+      <c r="B266" s="6">
+        <v>29</v>
+      </c>
       <c r="C266" s="7" t="s">
         <v>266</v>
       </c>
@@ -5060,7 +5482,9 @@
       <c r="A267" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B267" s="6"/>
+      <c r="B267" s="6">
+        <v>30</v>
+      </c>
       <c r="C267" s="7" t="s">
         <v>267</v>
       </c>
@@ -5072,7 +5496,9 @@
       <c r="A268" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B268" s="6"/>
+      <c r="B268" s="6">
+        <v>31</v>
+      </c>
       <c r="C268" s="7" t="s">
         <v>268</v>
       </c>
@@ -5084,7 +5510,9 @@
       <c r="A269" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B269" s="6"/>
+      <c r="B269" s="6">
+        <v>32</v>
+      </c>
       <c r="C269" s="7" t="s">
         <v>269</v>
       </c>
@@ -5096,7 +5524,9 @@
       <c r="A270" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B270" s="6"/>
+      <c r="B270" s="6">
+        <v>33</v>
+      </c>
       <c r="C270" s="7" t="s">
         <v>270</v>
       </c>
@@ -5108,7 +5538,9 @@
       <c r="A271" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B271" s="6"/>
+      <c r="B271" s="6">
+        <v>34</v>
+      </c>
       <c r="C271" s="7" t="s">
         <v>93</v>
       </c>
@@ -5120,7 +5552,9 @@
       <c r="A272" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B272" s="6"/>
+      <c r="B272" s="6">
+        <v>35</v>
+      </c>
       <c r="C272" s="7" t="s">
         <v>271</v>
       </c>
@@ -5140,7 +5574,9 @@
       <c r="A275" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B275" s="6"/>
+      <c r="B275" s="6">
+        <v>1</v>
+      </c>
       <c r="C275" s="7" t="s">
         <v>273</v>
       </c>
@@ -5152,7 +5588,9 @@
       <c r="A276" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B276" s="6"/>
+      <c r="B276" s="6">
+        <v>2</v>
+      </c>
       <c r="C276" s="7" t="s">
         <v>274</v>
       </c>
@@ -5164,7 +5602,9 @@
       <c r="A277" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B277" s="6"/>
+      <c r="B277" s="6">
+        <v>3</v>
+      </c>
       <c r="C277" s="7" t="s">
         <v>275</v>
       </c>
@@ -5176,7 +5616,9 @@
       <c r="A278" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B278" s="6"/>
+      <c r="B278" s="6">
+        <v>4</v>
+      </c>
       <c r="C278" s="7" t="s">
         <v>276</v>
       </c>
@@ -5188,7 +5630,9 @@
       <c r="A279" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B279" s="6"/>
+      <c r="B279" s="6">
+        <v>5</v>
+      </c>
       <c r="C279" s="7" t="s">
         <v>277</v>
       </c>
@@ -5200,7 +5644,9 @@
       <c r="A280" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B280" s="6"/>
+      <c r="B280" s="6">
+        <v>6</v>
+      </c>
       <c r="C280" s="7" t="s">
         <v>278</v>
       </c>
@@ -5212,7 +5658,9 @@
       <c r="A281" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B281" s="6"/>
+      <c r="B281" s="6">
+        <v>7</v>
+      </c>
       <c r="C281" s="7" t="s">
         <v>279</v>
       </c>
@@ -5224,7 +5672,9 @@
       <c r="A282" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B282" s="6"/>
+      <c r="B282" s="6">
+        <v>8</v>
+      </c>
       <c r="C282" s="7" t="s">
         <v>280</v>
       </c>
@@ -5236,7 +5686,9 @@
       <c r="A283" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B283" s="6"/>
+      <c r="B283" s="6">
+        <v>9</v>
+      </c>
       <c r="C283" s="7" t="s">
         <v>281</v>
       </c>
@@ -5248,7 +5700,9 @@
       <c r="A284" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B284" s="6"/>
+      <c r="B284" s="6">
+        <v>10</v>
+      </c>
       <c r="C284" s="7" t="s">
         <v>282</v>
       </c>
@@ -5260,7 +5714,9 @@
       <c r="A285" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B285" s="6"/>
+      <c r="B285" s="6">
+        <v>11</v>
+      </c>
       <c r="C285" s="7" t="s">
         <v>283</v>
       </c>
@@ -5272,7 +5728,9 @@
       <c r="A286" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B286" s="6"/>
+      <c r="B286" s="6">
+        <v>12</v>
+      </c>
       <c r="C286" s="7" t="s">
         <v>284</v>
       </c>
@@ -5284,7 +5742,9 @@
       <c r="A287" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B287" s="6"/>
+      <c r="B287" s="6">
+        <v>13</v>
+      </c>
       <c r="C287" s="7" t="s">
         <v>285</v>
       </c>
@@ -5296,7 +5756,9 @@
       <c r="A288" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B288" s="6"/>
+      <c r="B288" s="6">
+        <v>14</v>
+      </c>
       <c r="C288" s="7" t="s">
         <v>286</v>
       </c>
@@ -5308,7 +5770,9 @@
       <c r="A289" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B289" s="6"/>
+      <c r="B289" s="6">
+        <v>15</v>
+      </c>
       <c r="C289" s="7" t="s">
         <v>287</v>
       </c>
@@ -5320,7 +5784,9 @@
       <c r="A290" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B290" s="6"/>
+      <c r="B290" s="6">
+        <v>16</v>
+      </c>
       <c r="C290" s="7" t="s">
         <v>288</v>
       </c>
@@ -5332,7 +5798,9 @@
       <c r="A291" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B291" s="6"/>
+      <c r="B291" s="6">
+        <v>17</v>
+      </c>
       <c r="C291" s="7" t="s">
         <v>289</v>
       </c>
@@ -5344,7 +5812,9 @@
       <c r="A292" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B292" s="6"/>
+      <c r="B292" s="6">
+        <v>18</v>
+      </c>
       <c r="C292" s="7" t="s">
         <v>290</v>
       </c>
@@ -5356,7 +5826,9 @@
       <c r="A293" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="B293" s="6"/>
+      <c r="B293" s="6">
+        <v>19</v>
+      </c>
       <c r="C293" s="7" t="s">
         <v>291</v>
       </c>
@@ -5376,7 +5848,9 @@
       <c r="A296" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B296" s="6"/>
+      <c r="B296" s="6">
+        <v>1</v>
+      </c>
       <c r="C296" s="7" t="s">
         <v>293</v>
       </c>
@@ -5388,7 +5862,9 @@
       <c r="A297" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B297" s="6"/>
+      <c r="B297" s="6">
+        <v>2</v>
+      </c>
       <c r="C297" s="7" t="s">
         <v>294</v>
       </c>
@@ -5400,7 +5876,9 @@
       <c r="A298" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B298" s="6"/>
+      <c r="B298" s="6">
+        <v>3</v>
+      </c>
       <c r="C298" s="7" t="s">
         <v>295</v>
       </c>
@@ -5412,7 +5890,9 @@
       <c r="A299" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B299" s="6"/>
+      <c r="B299" s="6">
+        <v>4</v>
+      </c>
       <c r="C299" s="7" t="s">
         <v>296</v>
       </c>
@@ -5424,7 +5904,9 @@
       <c r="A300" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B300" s="6"/>
+      <c r="B300" s="6">
+        <v>5</v>
+      </c>
       <c r="C300" s="7" t="s">
         <v>297</v>
       </c>
@@ -5436,7 +5918,9 @@
       <c r="A301" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B301" s="6"/>
+      <c r="B301" s="6">
+        <v>6</v>
+      </c>
       <c r="C301" s="7" t="s">
         <v>298</v>
       </c>
@@ -5448,7 +5932,9 @@
       <c r="A302" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B302" s="6"/>
+      <c r="B302" s="6">
+        <v>7</v>
+      </c>
       <c r="C302" s="7" t="s">
         <v>299</v>
       </c>
@@ -5460,7 +5946,9 @@
       <c r="A303" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B303" s="6"/>
+      <c r="B303" s="6">
+        <v>8</v>
+      </c>
       <c r="C303" s="7" t="s">
         <v>300</v>
       </c>
@@ -5472,7 +5960,9 @@
       <c r="A304" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B304" s="6"/>
+      <c r="B304" s="6">
+        <v>9</v>
+      </c>
       <c r="C304" s="7" t="s">
         <v>301</v>
       </c>
@@ -5484,7 +5974,9 @@
       <c r="A305" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B305" s="6"/>
+      <c r="B305" s="6">
+        <v>10</v>
+      </c>
       <c r="C305" s="7" t="s">
         <v>302</v>
       </c>
@@ -5496,7 +5988,9 @@
       <c r="A306" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B306" s="6"/>
+      <c r="B306" s="6">
+        <v>11</v>
+      </c>
       <c r="C306" s="7" t="s">
         <v>303</v>
       </c>
@@ -5508,7 +6002,9 @@
       <c r="A307" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B307" s="6"/>
+      <c r="B307" s="6">
+        <v>12</v>
+      </c>
       <c r="C307" s="7" t="s">
         <v>304</v>
       </c>
@@ -5520,7 +6016,9 @@
       <c r="A308" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B308" s="6"/>
+      <c r="B308" s="6">
+        <v>13</v>
+      </c>
       <c r="C308" s="7" t="s">
         <v>305</v>
       </c>
@@ -5532,7 +6030,9 @@
       <c r="A309" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B309" s="6"/>
+      <c r="B309" s="6">
+        <v>14</v>
+      </c>
       <c r="C309" s="9" t="s">
         <v>306</v>
       </c>
@@ -5544,7 +6044,9 @@
       <c r="A310" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B310" s="6"/>
+      <c r="B310" s="6">
+        <v>15</v>
+      </c>
       <c r="C310" s="7" t="s">
         <v>307</v>
       </c>
@@ -5556,7 +6058,9 @@
       <c r="A311" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B311" s="6"/>
+      <c r="B311" s="6">
+        <v>16</v>
+      </c>
       <c r="C311" s="7" t="s">
         <v>308</v>
       </c>
@@ -5568,7 +6072,9 @@
       <c r="A312" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B312" s="6"/>
+      <c r="B312" s="6">
+        <v>17</v>
+      </c>
       <c r="C312" s="7" t="s">
         <v>309</v>
       </c>
@@ -5580,7 +6086,9 @@
       <c r="A313" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B313" s="6"/>
+      <c r="B313" s="6">
+        <v>18</v>
+      </c>
       <c r="C313" s="7" t="s">
         <v>310</v>
       </c>
@@ -5592,7 +6100,9 @@
       <c r="A314" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B314" s="6"/>
+      <c r="B314" s="6">
+        <v>19</v>
+      </c>
       <c r="C314" s="7" t="s">
         <v>311</v>
       </c>
@@ -5604,7 +6114,9 @@
       <c r="A315" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B315" s="6"/>
+      <c r="B315" s="6">
+        <v>20</v>
+      </c>
       <c r="C315" s="7" t="s">
         <v>312</v>
       </c>
@@ -5616,7 +6128,9 @@
       <c r="A316" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B316" s="6"/>
+      <c r="B316" s="6">
+        <v>21</v>
+      </c>
       <c r="C316" s="7" t="s">
         <v>313</v>
       </c>
@@ -5628,7 +6142,9 @@
       <c r="A317" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B317" s="6"/>
+      <c r="B317" s="6">
+        <v>22</v>
+      </c>
       <c r="C317" s="7" t="s">
         <v>314</v>
       </c>
@@ -5640,7 +6156,9 @@
       <c r="A318" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B318" s="6"/>
+      <c r="B318" s="6">
+        <v>23</v>
+      </c>
       <c r="C318" s="7" t="s">
         <v>315</v>
       </c>
@@ -5652,7 +6170,9 @@
       <c r="A319" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B319" s="6"/>
+      <c r="B319" s="6">
+        <v>24</v>
+      </c>
       <c r="C319" s="7" t="s">
         <v>316</v>
       </c>
@@ -5664,7 +6184,9 @@
       <c r="A320" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B320" s="6"/>
+      <c r="B320" s="6">
+        <v>25</v>
+      </c>
       <c r="C320" s="7" t="s">
         <v>317</v>
       </c>
@@ -5676,7 +6198,9 @@
       <c r="A321" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B321" s="6"/>
+      <c r="B321" s="6">
+        <v>26</v>
+      </c>
       <c r="C321" s="7" t="s">
         <v>318</v>
       </c>
@@ -5688,7 +6212,9 @@
       <c r="A322" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B322" s="6"/>
+      <c r="B322" s="6">
+        <v>27</v>
+      </c>
       <c r="C322" s="7" t="s">
         <v>319</v>
       </c>
@@ -5700,7 +6226,9 @@
       <c r="A323" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B323" s="6"/>
+      <c r="B323" s="6">
+        <v>28</v>
+      </c>
       <c r="C323" s="7" t="s">
         <v>320</v>
       </c>
@@ -5712,7 +6240,9 @@
       <c r="A324" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B324" s="6"/>
+      <c r="B324" s="6">
+        <v>29</v>
+      </c>
       <c r="C324" s="7" t="s">
         <v>321</v>
       </c>
@@ -5724,7 +6254,9 @@
       <c r="A325" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B325" s="6"/>
+      <c r="B325" s="6">
+        <v>30</v>
+      </c>
       <c r="C325" s="7" t="s">
         <v>322</v>
       </c>
@@ -5736,7 +6268,9 @@
       <c r="A326" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B326" s="6"/>
+      <c r="B326" s="6">
+        <v>31</v>
+      </c>
       <c r="C326" s="7" t="s">
         <v>323</v>
       </c>
@@ -5748,7 +6282,9 @@
       <c r="A327" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B327" s="6"/>
+      <c r="B327" s="6">
+        <v>32</v>
+      </c>
       <c r="C327" s="7" t="s">
         <v>324</v>
       </c>
@@ -5760,7 +6296,9 @@
       <c r="A328" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B328" s="6"/>
+      <c r="B328" s="6">
+        <v>33</v>
+      </c>
       <c r="C328" s="7" t="s">
         <v>325</v>
       </c>
@@ -5772,7 +6310,9 @@
       <c r="A329" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B329" s="6"/>
+      <c r="B329" s="6">
+        <v>34</v>
+      </c>
       <c r="C329" s="7" t="s">
         <v>326</v>
       </c>
@@ -5784,7 +6324,9 @@
       <c r="A330" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B330" s="6"/>
+      <c r="B330" s="6">
+        <v>35</v>
+      </c>
       <c r="C330" s="7" t="s">
         <v>327</v>
       </c>
@@ -5796,7 +6338,9 @@
       <c r="A331" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B331" s="6"/>
+      <c r="B331" s="6">
+        <v>36</v>
+      </c>
       <c r="C331" s="7" t="s">
         <v>328</v>
       </c>
@@ -5808,7 +6352,9 @@
       <c r="A332" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B332" s="6"/>
+      <c r="B332" s="6">
+        <v>37</v>
+      </c>
       <c r="C332" s="7" t="s">
         <v>329</v>
       </c>
@@ -5820,7 +6366,9 @@
       <c r="A333" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B333" s="6"/>
+      <c r="B333" s="6">
+        <v>38</v>
+      </c>
       <c r="C333" s="7" t="s">
         <v>330</v>
       </c>
@@ -5840,7 +6388,9 @@
       <c r="A336" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B336" s="6"/>
+      <c r="B336" s="6">
+        <v>1</v>
+      </c>
       <c r="C336" s="7" t="s">
         <v>332</v>
       </c>
@@ -5852,7 +6402,9 @@
       <c r="A337" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B337" s="6"/>
+      <c r="B337" s="6">
+        <v>2</v>
+      </c>
       <c r="C337" s="7" t="s">
         <v>333</v>
       </c>
@@ -5864,7 +6416,9 @@
       <c r="A338" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B338" s="6"/>
+      <c r="B338" s="6">
+        <v>3</v>
+      </c>
       <c r="C338" s="7" t="s">
         <v>334</v>
       </c>
@@ -5876,7 +6430,9 @@
       <c r="A339" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B339" s="6"/>
+      <c r="B339" s="6">
+        <v>4</v>
+      </c>
       <c r="C339" s="7" t="s">
         <v>335</v>
       </c>
@@ -5888,7 +6444,9 @@
       <c r="A340" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B340" s="6"/>
+      <c r="B340" s="6">
+        <v>5</v>
+      </c>
       <c r="C340" s="7" t="s">
         <v>336</v>
       </c>
@@ -5900,7 +6458,9 @@
       <c r="A341" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B341" s="6"/>
+      <c r="B341" s="6">
+        <v>6</v>
+      </c>
       <c r="C341" s="7" t="s">
         <v>337</v>
       </c>
@@ -5912,7 +6472,9 @@
       <c r="A342" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B342" s="6"/>
+      <c r="B342" s="6">
+        <v>7</v>
+      </c>
       <c r="C342" s="7" t="s">
         <v>338</v>
       </c>
@@ -5924,7 +6486,9 @@
       <c r="A343" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B343" s="6"/>
+      <c r="B343" s="6">
+        <v>8</v>
+      </c>
       <c r="C343" s="7" t="s">
         <v>339</v>
       </c>
@@ -5936,7 +6500,9 @@
       <c r="A344" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B344" s="6"/>
+      <c r="B344" s="6">
+        <v>9</v>
+      </c>
       <c r="C344" s="9" t="s">
         <v>340</v>
       </c>
@@ -5948,7 +6514,9 @@
       <c r="A345" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B345" s="6"/>
+      <c r="B345" s="6">
+        <v>10</v>
+      </c>
       <c r="C345" s="7" t="s">
         <v>341</v>
       </c>
@@ -5960,7 +6528,9 @@
       <c r="A346" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B346" s="6"/>
+      <c r="B346" s="6">
+        <v>11</v>
+      </c>
       <c r="C346" s="7" t="s">
         <v>342</v>
       </c>
@@ -5972,7 +6542,9 @@
       <c r="A347" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B347" s="6"/>
+      <c r="B347" s="6">
+        <v>12</v>
+      </c>
       <c r="C347" s="7" t="s">
         <v>343</v>
       </c>
@@ -5984,7 +6556,9 @@
       <c r="A348" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B348" s="6"/>
+      <c r="B348" s="6">
+        <v>13</v>
+      </c>
       <c r="C348" s="7" t="s">
         <v>344</v>
       </c>
@@ -5996,7 +6570,9 @@
       <c r="A349" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B349" s="6"/>
+      <c r="B349" s="6">
+        <v>14</v>
+      </c>
       <c r="C349" s="7" t="s">
         <v>345</v>
       </c>
@@ -6008,7 +6584,9 @@
       <c r="A350" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B350" s="6"/>
+      <c r="B350" s="6">
+        <v>15</v>
+      </c>
       <c r="C350" s="7" t="s">
         <v>346</v>
       </c>
@@ -6020,7 +6598,9 @@
       <c r="A351" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B351" s="6"/>
+      <c r="B351" s="6">
+        <v>16</v>
+      </c>
       <c r="C351" s="7" t="s">
         <v>347</v>
       </c>
@@ -6032,7 +6612,9 @@
       <c r="A352" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B352" s="6"/>
+      <c r="B352" s="6">
+        <v>17</v>
+      </c>
       <c r="C352" s="7" t="s">
         <v>348</v>
       </c>
@@ -6044,7 +6626,9 @@
       <c r="A353" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B353" s="6"/>
+      <c r="B353" s="6">
+        <v>18</v>
+      </c>
       <c r="C353" s="7" t="s">
         <v>349</v>
       </c>
@@ -6064,7 +6648,9 @@
       <c r="A356" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B356" s="6"/>
+      <c r="B356" s="6">
+        <v>1</v>
+      </c>
       <c r="C356" s="7" t="s">
         <v>351</v>
       </c>
@@ -6076,7 +6662,9 @@
       <c r="A357" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B357" s="6"/>
+      <c r="B357" s="6">
+        <v>2</v>
+      </c>
       <c r="C357" s="7" t="s">
         <v>352</v>
       </c>
@@ -6088,7 +6676,9 @@
       <c r="A358" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B358" s="6"/>
+      <c r="B358" s="6">
+        <v>3</v>
+      </c>
       <c r="C358" s="7" t="s">
         <v>353</v>
       </c>
@@ -6100,7 +6690,9 @@
       <c r="A359" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B359" s="6"/>
+      <c r="B359" s="6">
+        <v>4</v>
+      </c>
       <c r="C359" s="7" t="s">
         <v>354</v>
       </c>
@@ -6112,7 +6704,9 @@
       <c r="A360" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B360" s="6"/>
+      <c r="B360" s="6">
+        <v>5</v>
+      </c>
       <c r="C360" s="7" t="s">
         <v>355</v>
       </c>
@@ -6124,7 +6718,9 @@
       <c r="A361" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B361" s="6"/>
+      <c r="B361" s="6">
+        <v>6</v>
+      </c>
       <c r="C361" s="7" t="s">
         <v>356</v>
       </c>
@@ -6136,7 +6732,9 @@
       <c r="A362" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B362" s="6"/>
+      <c r="B362" s="6">
+        <v>7</v>
+      </c>
       <c r="C362" s="7" t="s">
         <v>357</v>
       </c>
@@ -6148,7 +6746,9 @@
       <c r="A363" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B363" s="6"/>
+      <c r="B363" s="6">
+        <v>8</v>
+      </c>
       <c r="C363" s="7" t="s">
         <v>358</v>
       </c>
@@ -6160,7 +6760,9 @@
       <c r="A364" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B364" s="6"/>
+      <c r="B364" s="6">
+        <v>9</v>
+      </c>
       <c r="C364" s="7" t="s">
         <v>359</v>
       </c>
@@ -6172,7 +6774,9 @@
       <c r="A365" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B365" s="6"/>
+      <c r="B365" s="6">
+        <v>10</v>
+      </c>
       <c r="C365" s="7" t="s">
         <v>360</v>
       </c>
@@ -6184,7 +6788,9 @@
       <c r="A366" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B366" s="6"/>
+      <c r="B366" s="6">
+        <v>11</v>
+      </c>
       <c r="C366" s="7" t="s">
         <v>361</v>
       </c>
@@ -6196,7 +6802,9 @@
       <c r="A367" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B367" s="6"/>
+      <c r="B367" s="6">
+        <v>12</v>
+      </c>
       <c r="C367" s="7" t="s">
         <v>362</v>
       </c>
@@ -6208,7 +6816,9 @@
       <c r="A368" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B368" s="6"/>
+      <c r="B368" s="6">
+        <v>13</v>
+      </c>
       <c r="C368" s="7" t="s">
         <v>363</v>
       </c>
@@ -6220,7 +6830,9 @@
       <c r="A369" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B369" s="6"/>
+      <c r="B369" s="6">
+        <v>14</v>
+      </c>
       <c r="C369" s="7" t="s">
         <v>364</v>
       </c>
@@ -6232,7 +6844,9 @@
       <c r="A370" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B370" s="6"/>
+      <c r="B370" s="6">
+        <v>15</v>
+      </c>
       <c r="C370" s="7" t="s">
         <v>365</v>
       </c>
@@ -6244,7 +6858,9 @@
       <c r="A371" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B371" s="6"/>
+      <c r="B371" s="6">
+        <v>16</v>
+      </c>
       <c r="C371" s="7" t="s">
         <v>366</v>
       </c>
@@ -6256,7 +6872,9 @@
       <c r="A372" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B372" s="6"/>
+      <c r="B372" s="6">
+        <v>17</v>
+      </c>
       <c r="C372" s="7" t="s">
         <v>367</v>
       </c>
@@ -6268,7 +6886,9 @@
       <c r="A373" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B373" s="6"/>
+      <c r="B373" s="6">
+        <v>18</v>
+      </c>
       <c r="C373" s="7" t="s">
         <v>368</v>
       </c>
@@ -6280,7 +6900,9 @@
       <c r="A374" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B374" s="6"/>
+      <c r="B374" s="6">
+        <v>19</v>
+      </c>
       <c r="C374" s="7" t="s">
         <v>369</v>
       </c>
@@ -6292,7 +6914,9 @@
       <c r="A375" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B375" s="6"/>
+      <c r="B375" s="6">
+        <v>20</v>
+      </c>
       <c r="C375" s="7" t="s">
         <v>370</v>
       </c>
@@ -6304,7 +6928,9 @@
       <c r="A376" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B376" s="6"/>
+      <c r="B376" s="6">
+        <v>21</v>
+      </c>
       <c r="C376" s="7" t="s">
         <v>371</v>
       </c>
@@ -6316,7 +6942,9 @@
       <c r="A377" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B377" s="6"/>
+      <c r="B377" s="6">
+        <v>22</v>
+      </c>
       <c r="C377" s="7" t="s">
         <v>372</v>
       </c>
@@ -6328,7 +6956,9 @@
       <c r="A378" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B378" s="6"/>
+      <c r="B378" s="6">
+        <v>23</v>
+      </c>
       <c r="C378" s="7" t="s">
         <v>373</v>
       </c>
@@ -6340,7 +6970,9 @@
       <c r="A379" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B379" s="6"/>
+      <c r="B379" s="6">
+        <v>24</v>
+      </c>
       <c r="C379" s="7" t="s">
         <v>374</v>
       </c>
@@ -6352,7 +6984,9 @@
       <c r="A380" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B380" s="6"/>
+      <c r="B380" s="6">
+        <v>25</v>
+      </c>
       <c r="C380" s="7" t="s">
         <v>375</v>
       </c>
@@ -6364,7 +6998,9 @@
       <c r="A381" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B381" s="6"/>
+      <c r="B381" s="6">
+        <v>26</v>
+      </c>
       <c r="C381" s="7" t="s">
         <v>376</v>
       </c>
@@ -6376,7 +7012,9 @@
       <c r="A382" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B382" s="6"/>
+      <c r="B382" s="6">
+        <v>27</v>
+      </c>
       <c r="C382" s="7" t="s">
         <v>377</v>
       </c>
@@ -6388,7 +7026,9 @@
       <c r="A383" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B383" s="6"/>
+      <c r="B383" s="6">
+        <v>28</v>
+      </c>
       <c r="C383" s="7" t="s">
         <v>378</v>
       </c>
@@ -6400,7 +7040,9 @@
       <c r="A384" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B384" s="6"/>
+      <c r="B384" s="6">
+        <v>29</v>
+      </c>
       <c r="C384" s="7" t="s">
         <v>379</v>
       </c>
@@ -6412,7 +7054,9 @@
       <c r="A385" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B385" s="6"/>
+      <c r="B385" s="6">
+        <v>30</v>
+      </c>
       <c r="C385" s="7" t="s">
         <v>380</v>
       </c>
@@ -6424,7 +7068,9 @@
       <c r="A386" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B386" s="6"/>
+      <c r="B386" s="6">
+        <v>31</v>
+      </c>
       <c r="C386" s="7" t="s">
         <v>381</v>
       </c>
@@ -6436,7 +7082,9 @@
       <c r="A387" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B387" s="6"/>
+      <c r="B387" s="6">
+        <v>32</v>
+      </c>
       <c r="C387" s="7" t="s">
         <v>382</v>
       </c>
@@ -6448,7 +7096,9 @@
       <c r="A388" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B388" s="6"/>
+      <c r="B388" s="6">
+        <v>33</v>
+      </c>
       <c r="C388" s="7" t="s">
         <v>383</v>
       </c>
@@ -6460,7 +7110,9 @@
       <c r="A389" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B389" s="6"/>
+      <c r="B389" s="6">
+        <v>34</v>
+      </c>
       <c r="C389" s="7" t="s">
         <v>384</v>
       </c>
@@ -6472,7 +7124,9 @@
       <c r="A390" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B390" s="6"/>
+      <c r="B390" s="6">
+        <v>35</v>
+      </c>
       <c r="C390" s="7" t="s">
         <v>384</v>
       </c>
@@ -6484,7 +7138,9 @@
       <c r="A391" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B391" s="6"/>
+      <c r="B391" s="6">
+        <v>36</v>
+      </c>
       <c r="C391" s="7" t="s">
         <v>385</v>
       </c>
@@ -6496,7 +7152,9 @@
       <c r="A392" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B392" s="6"/>
+      <c r="B392" s="6">
+        <v>37</v>
+      </c>
       <c r="C392" s="7" t="s">
         <v>386</v>
       </c>
@@ -6508,7 +7166,9 @@
       <c r="A393" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B393" s="6"/>
+      <c r="B393" s="6">
+        <v>38</v>
+      </c>
       <c r="C393" s="7" t="s">
         <v>387</v>
       </c>
@@ -6520,7 +7180,9 @@
       <c r="A394" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B394" s="6"/>
+      <c r="B394" s="6">
+        <v>39</v>
+      </c>
       <c r="C394" s="7" t="s">
         <v>388</v>
       </c>
@@ -6532,7 +7194,9 @@
       <c r="A395" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B395" s="6"/>
+      <c r="B395" s="6">
+        <v>40</v>
+      </c>
       <c r="C395" s="7" t="s">
         <v>389</v>
       </c>
@@ -6544,7 +7208,9 @@
       <c r="A396" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B396" s="6"/>
+      <c r="B396" s="6">
+        <v>41</v>
+      </c>
       <c r="C396" s="7" t="s">
         <v>390</v>
       </c>
@@ -6556,7 +7222,9 @@
       <c r="A397" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B397" s="6"/>
+      <c r="B397" s="6">
+        <v>42</v>
+      </c>
       <c r="C397" s="7" t="s">
         <v>391</v>
       </c>
@@ -6568,7 +7236,9 @@
       <c r="A398" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B398" s="6"/>
+      <c r="B398" s="6">
+        <v>43</v>
+      </c>
       <c r="C398" s="7" t="s">
         <v>392</v>
       </c>
@@ -6580,7 +7250,9 @@
       <c r="A399" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B399" s="6"/>
+      <c r="B399" s="6">
+        <v>44</v>
+      </c>
       <c r="C399" s="7" t="s">
         <v>393</v>
       </c>
@@ -6600,7 +7272,9 @@
       <c r="A402" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="B402" s="6"/>
+      <c r="B402" s="6">
+        <v>1</v>
+      </c>
       <c r="C402" s="7" t="s">
         <v>395</v>
       </c>
@@ -6612,7 +7286,9 @@
       <c r="A403" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="B403" s="6"/>
+      <c r="B403" s="6">
+        <v>2</v>
+      </c>
       <c r="C403" s="7" t="s">
         <v>396</v>
       </c>
@@ -6624,7 +7300,9 @@
       <c r="A404" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="B404" s="6"/>
+      <c r="B404" s="6">
+        <v>3</v>
+      </c>
       <c r="C404" s="7" t="s">
         <v>397</v>
       </c>
@@ -6636,7 +7314,9 @@
       <c r="A405" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="B405" s="6"/>
+      <c r="B405" s="6">
+        <v>4</v>
+      </c>
       <c r="C405" s="7" t="s">
         <v>95</v>
       </c>
@@ -6648,7 +7328,9 @@
       <c r="A406" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="B406" s="6"/>
+      <c r="B406" s="6">
+        <v>5</v>
+      </c>
       <c r="C406" s="7" t="s">
         <v>398</v>
       </c>
@@ -6660,7 +7342,9 @@
       <c r="A407" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="B407" s="6"/>
+      <c r="B407" s="6">
+        <v>6</v>
+      </c>
       <c r="C407" s="7" t="s">
         <v>399</v>
       </c>
@@ -6680,7 +7364,9 @@
       <c r="A410" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B410" s="6"/>
+      <c r="B410" s="6">
+        <v>1</v>
+      </c>
       <c r="C410" s="7" t="s">
         <v>401</v>
       </c>
@@ -6692,7 +7378,9 @@
       <c r="A411" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B411" s="6"/>
+      <c r="B411" s="6">
+        <v>2</v>
+      </c>
       <c r="C411" s="7" t="s">
         <v>402</v>
       </c>
@@ -6704,7 +7392,9 @@
       <c r="A412" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B412" s="6"/>
+      <c r="B412" s="6">
+        <v>3</v>
+      </c>
       <c r="C412" s="7" t="s">
         <v>403</v>
       </c>
@@ -6716,7 +7406,9 @@
       <c r="A413" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B413" s="6"/>
+      <c r="B413" s="6">
+        <v>4</v>
+      </c>
       <c r="C413" s="7" t="s">
         <v>404</v>
       </c>
@@ -6728,7 +7420,9 @@
       <c r="A414" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B414" s="6"/>
+      <c r="B414" s="6">
+        <v>5</v>
+      </c>
       <c r="C414" s="7" t="s">
         <v>405</v>
       </c>
@@ -6740,7 +7434,9 @@
       <c r="A415" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B415" s="6"/>
+      <c r="B415" s="6">
+        <v>6</v>
+      </c>
       <c r="C415" s="7" t="s">
         <v>406</v>
       </c>
@@ -6752,7 +7448,9 @@
       <c r="A416" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B416" s="6"/>
+      <c r="B416" s="6">
+        <v>7</v>
+      </c>
       <c r="C416" s="7" t="s">
         <v>407</v>
       </c>
@@ -6764,7 +7462,9 @@
       <c r="A417" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B417" s="6"/>
+      <c r="B417" s="6">
+        <v>8</v>
+      </c>
       <c r="C417" s="7" t="s">
         <v>280</v>
       </c>
@@ -6776,7 +7476,9 @@
       <c r="A418" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B418" s="6"/>
+      <c r="B418" s="6">
+        <v>9</v>
+      </c>
       <c r="C418" s="7" t="s">
         <v>408</v>
       </c>
@@ -6788,7 +7490,9 @@
       <c r="A419" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B419" s="6"/>
+      <c r="B419" s="6">
+        <v>10</v>
+      </c>
       <c r="C419" s="7" t="s">
         <v>409</v>
       </c>
@@ -6800,7 +7504,9 @@
       <c r="A420" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B420" s="6"/>
+      <c r="B420" s="6">
+        <v>11</v>
+      </c>
       <c r="C420" s="7" t="s">
         <v>410</v>
       </c>
@@ -6812,7 +7518,9 @@
       <c r="A421" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B421" s="6"/>
+      <c r="B421" s="6">
+        <v>12</v>
+      </c>
       <c r="C421" s="7" t="s">
         <v>411</v>
       </c>
@@ -6824,7 +7532,9 @@
       <c r="A422" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B422" s="6"/>
+      <c r="B422" s="6">
+        <v>13</v>
+      </c>
       <c r="C422" s="7" t="s">
         <v>412</v>
       </c>
@@ -6836,7 +7546,9 @@
       <c r="A423" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B423" s="6"/>
+      <c r="B423" s="6">
+        <v>14</v>
+      </c>
       <c r="C423" s="7" t="s">
         <v>413</v>
       </c>
@@ -6848,7 +7560,9 @@
       <c r="A424" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B424" s="6"/>
+      <c r="B424" s="6">
+        <v>15</v>
+      </c>
       <c r="C424" s="7" t="s">
         <v>414</v>
       </c>
@@ -6860,7 +7574,9 @@
       <c r="A425" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B425" s="6"/>
+      <c r="B425" s="6">
+        <v>16</v>
+      </c>
       <c r="C425" s="7" t="s">
         <v>415</v>
       </c>
@@ -6872,7 +7588,9 @@
       <c r="A426" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B426" s="6"/>
+      <c r="B426" s="6">
+        <v>17</v>
+      </c>
       <c r="C426" s="7" t="s">
         <v>416</v>
       </c>
@@ -6884,7 +7602,9 @@
       <c r="A427" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B427" s="6"/>
+      <c r="B427" s="6">
+        <v>18</v>
+      </c>
       <c r="C427" s="7" t="s">
         <v>417</v>
       </c>
@@ -6896,7 +7616,9 @@
       <c r="A428" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B428" s="6"/>
+      <c r="B428" s="6">
+        <v>19</v>
+      </c>
       <c r="C428" s="7" t="s">
         <v>418</v>
       </c>
@@ -6908,7 +7630,9 @@
       <c r="A429" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B429" s="6"/>
+      <c r="B429" s="6">
+        <v>20</v>
+      </c>
       <c r="C429" s="7" t="s">
         <v>419</v>
       </c>
@@ -6920,7 +7644,9 @@
       <c r="A430" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B430" s="6"/>
+      <c r="B430" s="6">
+        <v>21</v>
+      </c>
       <c r="C430" s="7" t="s">
         <v>420</v>
       </c>
@@ -6932,7 +7658,9 @@
       <c r="A431" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B431" s="6"/>
+      <c r="B431" s="6">
+        <v>22</v>
+      </c>
       <c r="C431" s="7" t="s">
         <v>421</v>
       </c>
@@ -6944,7 +7672,9 @@
       <c r="A432" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B432" s="6"/>
+      <c r="B432" s="6">
+        <v>23</v>
+      </c>
       <c r="C432" s="7" t="s">
         <v>422</v>
       </c>
@@ -6956,7 +7686,9 @@
       <c r="A433" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B433" s="6"/>
+      <c r="B433" s="6">
+        <v>24</v>
+      </c>
       <c r="C433" s="7" t="s">
         <v>423</v>
       </c>
@@ -6968,7 +7700,9 @@
       <c r="A434" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B434" s="6"/>
+      <c r="B434" s="6">
+        <v>25</v>
+      </c>
       <c r="C434" s="7" t="s">
         <v>424</v>
       </c>
@@ -6980,7 +7714,9 @@
       <c r="A435" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B435" s="6"/>
+      <c r="B435" s="6">
+        <v>26</v>
+      </c>
       <c r="C435" s="7" t="s">
         <v>425</v>
       </c>
@@ -6992,7 +7728,9 @@
       <c r="A436" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B436" s="6"/>
+      <c r="B436" s="6">
+        <v>27</v>
+      </c>
       <c r="C436" s="7" t="s">
         <v>426</v>
       </c>
@@ -7004,7 +7742,9 @@
       <c r="A437" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B437" s="6"/>
+      <c r="B437" s="6">
+        <v>28</v>
+      </c>
       <c r="C437" s="7" t="s">
         <v>427</v>
       </c>
@@ -7016,7 +7756,9 @@
       <c r="A438" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B438" s="6"/>
+      <c r="B438" s="6">
+        <v>29</v>
+      </c>
       <c r="C438" s="7" t="s">
         <v>428</v>
       </c>
@@ -7028,7 +7770,9 @@
       <c r="A439" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B439" s="6"/>
+      <c r="B439" s="6">
+        <v>30</v>
+      </c>
       <c r="C439" s="7" t="s">
         <v>429</v>
       </c>
@@ -7040,7 +7784,9 @@
       <c r="A440" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B440" s="6"/>
+      <c r="B440" s="6">
+        <v>31</v>
+      </c>
       <c r="C440" s="7" t="s">
         <v>430</v>
       </c>
@@ -7052,7 +7798,9 @@
       <c r="A441" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B441" s="6"/>
+      <c r="B441" s="6">
+        <v>32</v>
+      </c>
       <c r="C441" s="7" t="s">
         <v>431</v>
       </c>
@@ -7064,7 +7812,9 @@
       <c r="A442" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B442" s="6"/>
+      <c r="B442" s="6">
+        <v>33</v>
+      </c>
       <c r="C442" s="7" t="s">
         <v>432</v>
       </c>
@@ -7076,7 +7826,9 @@
       <c r="A443" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B443" s="6"/>
+      <c r="B443" s="6">
+        <v>34</v>
+      </c>
       <c r="C443" s="7" t="s">
         <v>433</v>
       </c>
@@ -7088,7 +7840,9 @@
       <c r="A444" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B444" s="6"/>
+      <c r="B444" s="6">
+        <v>35</v>
+      </c>
       <c r="C444" s="7" t="s">
         <v>434</v>
       </c>
@@ -7100,7 +7854,9 @@
       <c r="A445" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B445" s="6"/>
+      <c r="B445" s="6">
+        <v>36</v>
+      </c>
       <c r="C445" s="7" t="s">
         <v>435</v>
       </c>
@@ -7112,7 +7868,9 @@
       <c r="A446" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B446" s="6"/>
+      <c r="B446" s="6">
+        <v>37</v>
+      </c>
       <c r="C446" s="7" t="s">
         <v>436</v>
       </c>
@@ -7124,7 +7882,9 @@
       <c r="A447" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B447" s="6"/>
+      <c r="B447" s="6">
+        <v>38</v>
+      </c>
       <c r="C447" s="7" t="s">
         <v>437</v>
       </c>
@@ -7136,7 +7896,9 @@
       <c r="A448" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B448" s="6"/>
+      <c r="B448" s="6">
+        <v>39</v>
+      </c>
       <c r="C448" s="7" t="s">
         <v>438</v>
       </c>
@@ -7148,7 +7910,9 @@
       <c r="A449" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B449" s="6"/>
+      <c r="B449" s="6">
+        <v>40</v>
+      </c>
       <c r="C449" s="7" t="s">
         <v>439</v>
       </c>
@@ -7160,7 +7924,9 @@
       <c r="A450" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B450" s="6"/>
+      <c r="B450" s="6">
+        <v>41</v>
+      </c>
       <c r="C450" s="7" t="s">
         <v>440</v>
       </c>
@@ -7172,7 +7938,9 @@
       <c r="A451" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B451" s="6"/>
+      <c r="B451" s="6">
+        <v>42</v>
+      </c>
       <c r="C451" s="7" t="s">
         <v>441</v>
       </c>
@@ -7184,7 +7952,9 @@
       <c r="A452" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B452" s="6"/>
+      <c r="B452" s="6">
+        <v>43</v>
+      </c>
       <c r="C452" s="7" t="s">
         <v>442</v>
       </c>
@@ -7196,7 +7966,9 @@
       <c r="A453" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B453" s="6"/>
+      <c r="B453" s="6">
+        <v>44</v>
+      </c>
       <c r="C453" s="7" t="s">
         <v>443</v>
       </c>
@@ -7208,7 +7980,9 @@
       <c r="A454" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B454" s="6"/>
+      <c r="B454" s="6">
+        <v>45</v>
+      </c>
       <c r="C454" s="7" t="s">
         <v>444</v>
       </c>
@@ -7220,7 +7994,9 @@
       <c r="A455" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B455" s="6"/>
+      <c r="B455" s="6">
+        <v>46</v>
+      </c>
       <c r="C455" s="7" t="s">
         <v>445</v>
       </c>
@@ -7232,7 +8008,9 @@
       <c r="A456" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B456" s="6"/>
+      <c r="B456" s="6">
+        <v>47</v>
+      </c>
       <c r="C456" s="7" t="s">
         <v>446</v>
       </c>
@@ -7244,7 +8022,9 @@
       <c r="A457" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B457" s="6"/>
+      <c r="B457" s="6">
+        <v>48</v>
+      </c>
       <c r="C457" s="7" t="s">
         <v>447</v>
       </c>
@@ -7256,7 +8036,9 @@
       <c r="A458" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B458" s="6"/>
+      <c r="B458" s="6">
+        <v>49</v>
+      </c>
       <c r="C458" s="7" t="s">
         <v>448</v>
       </c>
@@ -7268,7 +8050,9 @@
       <c r="A459" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B459" s="6"/>
+      <c r="B459" s="6">
+        <v>50</v>
+      </c>
       <c r="C459" s="7" t="s">
         <v>449</v>
       </c>
@@ -7280,7 +8064,9 @@
       <c r="A460" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B460" s="6"/>
+      <c r="B460" s="6">
+        <v>51</v>
+      </c>
       <c r="C460" s="7" t="s">
         <v>450</v>
       </c>
@@ -7292,7 +8078,9 @@
       <c r="A461" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B461" s="6"/>
+      <c r="B461" s="6">
+        <v>52</v>
+      </c>
       <c r="C461" s="7" t="s">
         <v>451</v>
       </c>
@@ -7304,7 +8092,9 @@
       <c r="A462" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B462" s="6"/>
+      <c r="B462" s="6">
+        <v>53</v>
+      </c>
       <c r="C462" s="7" t="s">
         <v>452</v>
       </c>
@@ -7316,7 +8106,9 @@
       <c r="A463" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B463" s="6"/>
+      <c r="B463" s="6">
+        <v>54</v>
+      </c>
       <c r="C463" s="7" t="s">
         <v>453</v>
       </c>
@@ -7328,7 +8120,9 @@
       <c r="A464" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B464" s="6"/>
+      <c r="B464" s="6">
+        <v>55</v>
+      </c>
       <c r="C464" s="7" t="s">
         <v>454</v>
       </c>
@@ -7340,7 +8134,9 @@
       <c r="A465" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B465" s="6"/>
+      <c r="B465" s="6">
+        <v>56</v>
+      </c>
       <c r="C465" s="7" t="s">
         <v>455</v>
       </c>
@@ -7352,7 +8148,9 @@
       <c r="A466" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B466" s="6"/>
+      <c r="B466" s="6">
+        <v>57</v>
+      </c>
       <c r="C466" s="7" t="s">
         <v>456</v>
       </c>
@@ -7364,7 +8162,9 @@
       <c r="A467" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B467" s="6"/>
+      <c r="B467" s="6">
+        <v>58</v>
+      </c>
       <c r="C467" s="7" t="s">
         <v>457</v>
       </c>
@@ -7376,7 +8176,9 @@
       <c r="A468" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B468" s="6"/>
+      <c r="B468" s="6">
+        <v>59</v>
+      </c>
       <c r="C468" s="7" t="s">
         <v>458</v>
       </c>
@@ -7388,7 +8190,9 @@
       <c r="A469" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B469" s="6"/>
+      <c r="B469" s="6">
+        <v>60</v>
+      </c>
       <c r="C469" s="7" t="s">
         <v>459</v>
       </c>
@@ -7410,7 +8214,9 @@
       <c r="A472" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="B472" s="6"/>
+      <c r="B472" s="6">
+        <v>1</v>
+      </c>
       <c r="C472" s="7" t="s">
         <v>461</v>
       </c>
@@ -7422,7 +8228,9 @@
       <c r="A473" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="B473" s="6"/>
+      <c r="B473" s="6">
+        <v>2</v>
+      </c>
       <c r="C473" s="7" t="s">
         <v>462</v>
       </c>
@@ -7434,7 +8242,9 @@
       <c r="A474" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="B474" s="6"/>
+      <c r="B474" s="6">
+        <v>3</v>
+      </c>
       <c r="C474" s="7" t="s">
         <v>463</v>
       </c>
@@ -7446,7 +8256,9 @@
       <c r="A475" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="B475" s="6"/>
+      <c r="B475" s="6">
+        <v>4</v>
+      </c>
       <c r="C475" s="7" t="s">
         <v>464</v>
       </c>
@@ -7458,7 +8270,9 @@
       <c r="A476" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="B476" s="6"/>
+      <c r="B476" s="6">
+        <v>5</v>
+      </c>
       <c r="C476" s="7" t="s">
         <v>465</v>
       </c>
@@ -7470,7 +8284,9 @@
       <c r="A477" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="B477" s="6"/>
+      <c r="B477" s="6">
+        <v>6</v>
+      </c>
       <c r="C477" s="7" t="s">
         <v>466</v>
       </c>
@@ -7482,7 +8298,9 @@
       <c r="A478" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="B478" s="6"/>
+      <c r="B478" s="6">
+        <v>7</v>
+      </c>
       <c r="C478" s="7" t="s">
         <v>467</v>
       </c>
@@ -7494,7 +8312,9 @@
       <c r="A479" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="B479" s="6"/>
+      <c r="B479" s="6">
+        <v>8</v>
+      </c>
       <c r="C479" s="7" t="s">
         <v>468</v>
       </c>
@@ -7506,7 +8326,9 @@
       <c r="A480" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="B480" s="6"/>
+      <c r="B480" s="6">
+        <v>9</v>
+      </c>
       <c r="C480" s="7" t="s">
         <v>469</v>
       </c>
@@ -7518,7 +8340,9 @@
       <c r="A481" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="B481" s="6"/>
+      <c r="B481" s="6">
+        <v>10</v>
+      </c>
       <c r="C481" s="7" t="s">
         <v>470</v>
       </c>

</xml_diff>

<commit_message>
count set bits from 1 to n
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\vineet\Coding\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86C1EAA-0268-4614-9681-1D9737BB78A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A668CAF-3652-47B0-AA24-3E03A95FDD3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8263,7 +8263,7 @@
         <v>464</v>
       </c>
       <c r="D475" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="476" spans="1:4" ht="21">

</xml_diff>

<commit_message>
max rectangle in matrix
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\vineet\Coding\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A668CAF-3652-47B0-AA24-3E03A95FDD3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210942A1-B5D7-441A-9B35-E60F7BDCEAD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1927,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A466" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D475" sqref="D475"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
@@ -2565,7 +2565,7 @@
         <v>54</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Common elements in matrix
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\vineet\Coding\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210942A1-B5D7-441A-9B35-E60F7BDCEAD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17DB695-07CA-4CE6-885F-97DA457A90B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1927,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
@@ -2579,7 +2579,7 @@
         <v>55</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="21">
@@ -2621,7 +2621,7 @@
         <v>58</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="21">

</xml_diff>